<commit_message>
Additional results for peer review
</commit_message>
<xml_diff>
--- a/table_s2_real_read_results.xlsx
+++ b/table_s2_real_read_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Dropbox/Uni_research/Projects/Trycycler/Paper_GitHub_repo/2_real_read_tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Dropbox/Uni_research/Projects/Trycycler/PAPER/GitHub_repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FFC8FD-BBDE-3449-B9B7-0B3AF8EDC50E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9293FA6C-44FF-6B45-B294-43D2A9F144F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3280" yWindow="-23520" windowWidth="36200" windowHeight="19000" xr2:uid="{735A4778-CFAE-5E49-9105-BF0324A3A577}"/>
+    <workbookView xWindow="-2040" yWindow="-24920" windowWidth="43740" windowHeight="19000" xr2:uid="{735A4778-CFAE-5E49-9105-BF0324A3A577}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet descriptions" sheetId="14" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="IDEEL results" sheetId="10" r:id="rId11"/>
     <sheet name="IDEEL results (fixed circ)" sheetId="11" r:id="rId12"/>
     <sheet name="Repeat identities" sheetId="13" r:id="rId13"/>
+    <sheet name="Medaka order" sheetId="21" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -170,6 +171,42 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={D566289C-92B8-A840-9B9C-2BA8ECE3BEF2}</author>
+    <author>tc={4DEB7657-53F0-1D4B-908A-F222C621892D}</author>
+    <author>tc={DCD486FB-9D3B-3941-8DFC-8FF860561C8E}</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{D566289C-92B8-A840-9B9C-2BA8ECE3BEF2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This followed the standard approach recommended in the documentation: running Trycycler and then Medaka on a per-replicon basis.</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{4DEB7657-53F0-1D4B-908A-F222C621892D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    In this approach I ran Medaka on each of Trycycler’s input assemblies, using the same subsampled reads as were used to make the input assemblies. I then did not run Medaka on the final result.</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="2" shapeId="0" xr:uid="{DCD486FB-9D3B-3941-8DFC-8FF860561C8E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This approach used both of the previous methods: running Medaka on Trycycler’s input assemblies, then running Medaka on the final Trycycler contigs on a per-replicon basis.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
@@ -193,7 +230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="139">
   <si>
     <t>yes</t>
   </si>
@@ -1556,6 +1593,46 @@
   <si>
     <t>Assembly</t>
   </si>
+  <si>
+    <t>Medaka
++Trycycler
+A vs B</t>
+  </si>
+  <si>
+    <t>Medaka
++Trycycler
++Medaka
+A vs B</t>
+  </si>
+  <si>
+    <t>Qscore</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Medaka order</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> worksheet contains results (same format as the Comparisons worksheet) for a few different orders of running Trycycler and Medaka.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1567,7 +1644,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1647,6 +1724,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -2048,7 +2131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="445">
+  <cellXfs count="450">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2946,6 +3029,13 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3328,9 +3418,23 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B1" dT="2021-08-18T04:46:08.10" personId="{266805F7-B702-E34C-B082-D75EC3CBF74C}" id="{D566289C-92B8-A840-9B9C-2BA8ECE3BEF2}">
+    <text>This followed the standard approach recommended in the documentation: running Trycycler and then Medaka on a per-replicon basis.</text>
+  </threadedComment>
+  <threadedComment ref="E1" dT="2021-08-18T04:46:54.72" personId="{266805F7-B702-E34C-B082-D75EC3CBF74C}" id="{4DEB7657-53F0-1D4B-908A-F222C621892D}">
+    <text>In this approach I ran Medaka on each of Trycycler’s input assemblies, using the same subsampled reads as were used to make the input assemblies. I then did not run Medaka on the final result.</text>
+  </threadedComment>
+  <threadedComment ref="H1" dT="2021-08-18T04:47:38.17" personId="{266805F7-B702-E34C-B082-D75EC3CBF74C}" id="{DCD486FB-9D3B-3941-8DFC-8FF860561C8E}">
+    <text>This approach used both of the previous methods: running Medaka on Trycycler’s input assemblies, then running Medaka on the final Trycycler contigs on a per-replicon basis.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA2C5122-E092-B144-9BE5-99209615D2DE}">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3402,6 +3506,11 @@
         <v>64</v>
       </c>
     </row>
+    <row r="25" spans="1:1" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="256" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3411,9 +3520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4ADF486-198A-FE48-AF68-367F940EDA37}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3850,9 +3957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC59EB6-D5B8-DD4D-AAB8-37B225D7D721}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4560,7 +4665,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U28" sqref="U28"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5836,21 +5941,324 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="AL1:AO1"/>
     <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="C9 E9 G9 I9 K9 M9 O9 Q9 S9 U9 W9 Y9 AA9:AO9" formula="1"/>
   </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0097C334-DA2E-DB4A-A1E1-E62B08DD7239}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" style="149" customWidth="1"/>
+    <col min="3" max="3" width="9" style="449" customWidth="1"/>
+    <col min="4" max="4" width="9" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="149" customWidth="1"/>
+    <col min="6" max="6" width="9" style="449" customWidth="1"/>
+    <col min="7" max="7" width="9" style="7" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="149" customWidth="1"/>
+    <col min="9" max="9" width="9" style="449" customWidth="1"/>
+    <col min="10" max="10" width="9" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="85" customFormat="1" ht="79" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="435" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="429"/>
+      <c r="D1" s="430"/>
+      <c r="E1" s="435" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="429"/>
+      <c r="G1" s="430"/>
+      <c r="H1" s="435" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" s="429"/>
+      <c r="J1" s="430"/>
+      <c r="K1" s="20"/>
+    </row>
+    <row r="2" spans="1:11" s="86" customFormat="1" ht="62" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="150" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="445" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="89" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="150" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="445" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" s="89" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="146" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="445" t="s">
+        <v>137</v>
+      </c>
+      <c r="J2" s="90" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="91"/>
+    </row>
+    <row r="3" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="151">
+        <v>0.99997950000000002</v>
+      </c>
+      <c r="C3" s="446">
+        <f>IF(B3=1,"inf",-10*LOG10(1-B3))</f>
+        <v>46.882461389446931</v>
+      </c>
+      <c r="D3" s="83">
+        <v>0.98</v>
+      </c>
+      <c r="E3" s="151">
+        <v>0.99997100000000005</v>
+      </c>
+      <c r="F3" s="446">
+        <f>IF(E3=1,"inf",-10*LOG10(1-E3))</f>
+        <v>45.376020021018562</v>
+      </c>
+      <c r="G3" s="83">
+        <v>0.98</v>
+      </c>
+      <c r="H3" s="147">
+        <v>0.9999789</v>
+      </c>
+      <c r="I3" s="446">
+        <f>IF(H3=1,"inf",-10*LOG10(1-H3))</f>
+        <v>46.757175447023869</v>
+      </c>
+      <c r="J3" s="83">
+        <v>0.98</v>
+      </c>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="152">
+        <v>0.99995920000000005</v>
+      </c>
+      <c r="C4" s="447">
+        <f>IF(B4=1,"inf",-10*LOG10(1-B4))</f>
+        <v>43.893398369106308</v>
+      </c>
+      <c r="D4" s="84">
+        <v>0.97</v>
+      </c>
+      <c r="E4" s="152">
+        <v>0.9999422</v>
+      </c>
+      <c r="F4" s="447">
+        <f>IF(E4=1,"inf",-10*LOG10(1-E4))</f>
+        <v>42.380721615794954</v>
+      </c>
+      <c r="G4" s="84">
+        <v>0.98</v>
+      </c>
+      <c r="H4" s="148">
+        <v>0.99995230000000002</v>
+      </c>
+      <c r="I4" s="447">
+        <f>IF(H4=1,"inf",-10*LOG10(1-H4))</f>
+        <v>43.214816209600329</v>
+      </c>
+      <c r="J4" s="84">
+        <v>0.98</v>
+      </c>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="152">
+        <v>0.99983569999999999</v>
+      </c>
+      <c r="C5" s="447">
+        <f>IF(B5=1,"inf",-10*LOG10(1-B5))</f>
+        <v>37.843624365649219</v>
+      </c>
+      <c r="D5" s="84">
+        <v>0.97</v>
+      </c>
+      <c r="E5" s="152">
+        <v>0.99982839999999995</v>
+      </c>
+      <c r="F5" s="447">
+        <f>IF(E5=1,"inf",-10*LOG10(1-E5))</f>
+        <v>37.654827164871882</v>
+      </c>
+      <c r="G5" s="84">
+        <v>0.97</v>
+      </c>
+      <c r="H5" s="148">
+        <v>0.99983339999999998</v>
+      </c>
+      <c r="I5" s="447">
+        <f>IF(H5=1,"inf",-10*LOG10(1-H5))</f>
+        <v>37.783250029291878</v>
+      </c>
+      <c r="J5" s="84">
+        <v>0.97</v>
+      </c>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="152">
+        <v>0.9999401</v>
+      </c>
+      <c r="C6" s="447">
+        <f>IF(B6=1,"inf",-10*LOG10(1-B6))</f>
+        <v>42.22573177610677</v>
+      </c>
+      <c r="D6" s="84">
+        <v>0.96</v>
+      </c>
+      <c r="E6" s="152">
+        <v>0.99992639999999999</v>
+      </c>
+      <c r="F6" s="447">
+        <f>IF(E6=1,"inf",-10*LOG10(1-E6))</f>
+        <v>41.331221856624595</v>
+      </c>
+      <c r="G6" s="84">
+        <v>0.96</v>
+      </c>
+      <c r="H6" s="148">
+        <v>0.99993810000000005</v>
+      </c>
+      <c r="I6" s="447">
+        <f>IF(H6=1,"inf",-10*LOG10(1-H6))</f>
+        <v>42.083093509802467</v>
+      </c>
+      <c r="J6" s="84">
+        <v>0.96</v>
+      </c>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="152">
+        <v>0.99995040000000002</v>
+      </c>
+      <c r="C7" s="447">
+        <f>IF(B7=1,"inf",-10*LOG10(1-B7))</f>
+        <v>43.045183235099515</v>
+      </c>
+      <c r="D7" s="84">
+        <v>0.97</v>
+      </c>
+      <c r="E7" s="152">
+        <v>0.99993949999999998</v>
+      </c>
+      <c r="F7" s="447">
+        <f>IF(E7=1,"inf",-10*LOG10(1-E7))</f>
+        <v>42.182446253473955</v>
+      </c>
+      <c r="G7" s="84">
+        <v>0.98</v>
+      </c>
+      <c r="H7" s="148">
+        <v>0.99994499999999997</v>
+      </c>
+      <c r="I7" s="447">
+        <f>IF(H7=1,"inf",-10*LOG10(1-H7))</f>
+        <v>42.596373105055406</v>
+      </c>
+      <c r="J7" s="84">
+        <v>0.98</v>
+      </c>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="264">
+        <v>0.99994150000000004</v>
+      </c>
+      <c r="C8" s="448">
+        <f>IF(B8=1,"inf",-10*LOG10(1-B8))</f>
+        <v>42.328441339181062</v>
+      </c>
+      <c r="D8" s="265">
+        <v>0.97</v>
+      </c>
+      <c r="E8" s="264">
+        <v>0.99994130000000003</v>
+      </c>
+      <c r="F8" s="448">
+        <f>IF(E8=1,"inf",-10*LOG10(1-E8))</f>
+        <v>42.313618987526283</v>
+      </c>
+      <c r="G8" s="265">
+        <v>0.97</v>
+      </c>
+      <c r="H8" s="266">
+        <v>0.99994059999999996</v>
+      </c>
+      <c r="I8" s="448">
+        <f>IF(H8=1,"inf",-10*LOG10(1-H8))</f>
+        <v>42.262135550184937</v>
+      </c>
+      <c r="J8" s="265">
+        <v>0.97</v>
+      </c>
+      <c r="K8" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6824,7 +7232,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P17" sqref="P17"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8399,10 +8807,10 @@
   <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AF3" sqref="AF3:AF8"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9214,9 +9622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E52B5EA-0D5A-5747-9340-A15820583CFB}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9569,9 +9975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D78D6E-B6BF-D34C-B305-5A0C63E37AEC}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9924,9 +10328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0ECAD0C-E9D1-9E42-833D-C7863B16B8EF}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>